<commit_message>
Update reference to ClosedXml in Samples project
</commit_message>
<xml_diff>
--- a/ExcelReportGenerator.Samples/Reports/Templates/GroupingWithPanelHierarchy.xlsx
+++ b/ExcelReportGenerator.Samples/Reports/Templates/GroupingWithPanelHierarchy.xlsx
@@ -359,13 +359,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,7 +671,7 @@
   <dimension ref="A2:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:R2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,11 +857,10 @@
       <c r="B10" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B2:R2"/>
     <mergeCell ref="B3:R3"/>
-    <mergeCell ref="C7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>